<commit_message>
added the handling of the winner
</commit_message>
<xml_diff>
--- a/tournament_BDF 12.xlsx
+++ b/tournament_BDF 12.xlsx
@@ -471,22 +471,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t xml:space="preserve">Test </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>09:26</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>TEst 1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>09:21</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>TEst 2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -495,17 +495,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TEst 3</t>
+          <t>Test 3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:26</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>TEst 2</t>
+          <t>Test 4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -519,17 +519,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TEst 2</t>
+          <t>Test 4</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:26</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TEst 4</t>
+          <t>TEst 1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -543,23 +543,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TEst 4</t>
+          <t>TEst 1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:26</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>TEst 4</t>
+          <t>WINNER</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
better handling of the eliminations
</commit_message>
<xml_diff>
--- a/tournament_BDF 12.xlsx
+++ b/tournament_BDF 12.xlsx
@@ -471,17 +471,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Test </t>
+          <t>TEst 2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>09:26</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>TEst 1</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -495,17 +495,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Test 3</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09:26</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Test 4</t>
+          <t>TEst 3</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -519,22 +519,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Test 4</t>
+          <t>TEst 3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>09:26</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TEst 1</t>
+          <t>TEst4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -543,12 +543,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TEst 1</t>
+          <t>TEst4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>09:26</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">

</xml_diff>